<commit_message>
pre stu comment qa
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheets/alert-initiator.xlsx
+++ b/input/resources-spreadsheets/alert-initiator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-alerts/input/resources-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7DFDB2-03DF-E44F-B8CB-50689B1323C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1692159C-10B2-A146-A462-BDBC9759980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46320" yWindow="500" windowWidth="31900" windowHeight="27460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68300" yWindow="500" windowWidth="31900" windowHeight="27460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capstatements" sheetId="14" r:id="rId1"/>
@@ -49,6 +49,25 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={A131816A-C462-0347-A84D-A3474CA26673}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{A131816A-C462-0347-A84D-A3474CA26673}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is used to to get ig data a and load updated cap statement
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>User</author>
   </authors>
   <commentList>
@@ -676,7 +695,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +791,12 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -818,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -848,7 +873,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -865,6 +889,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Eric Haas" id="{41572270-CD8D-7642-8D79-E846A5EE2254}" userId="deea5e002be8d274" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1162,6 +1192,15 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2024-12-07T01:00:46.99" personId="{41572270-CD8D-7642-8D79-E846A5EE2254}" id="{A131816A-C462-0347-A84D-A3474CA26673}">
+    <text xml:space="preserve">This is used to to get ig data a and load updated cap statement
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80AEECE6-462E-BC49-B086-7EFF1E6B2200}">
   <sheetPr codeName="Sheet1"/>
@@ -2272,7 +2311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FE7B3C-655A-420A-A582-37B1D34DD578}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FE7B3C-655A-420A-A582-37B1D34DD578}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -2305,7 +2344,7 @@
       <c r="A3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2359,6 +2398,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update change log and whats new for comment publication
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheets/alert-initiator.xlsx
+++ b/input/resources-spreadsheets/alert-initiator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-alerts/input/resources-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1692159C-10B2-A146-A462-BDBC9759980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A114D6-ABFE-6F42-B20D-1D8258D31345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68300" yWindow="500" windowWidth="31900" windowHeight="27460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68300" yWindow="500" windowWidth="31900" windowHeight="27460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capstatements" sheetId="14" r:id="rId1"/>
@@ -363,11 +363,6 @@
     <t>client</t>
   </si>
   <si>
-    <t xml:space="preserve">1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
-1. For security considerations specific to this guide refer to the  [Security](security.html) page for requirements and recommendations.
-</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
@@ -690,12 +685,17 @@
   <si>
     <t>https://build.fhir.org/ig/HL7/davinci-alerts/package.tgz</t>
   </si>
+  <si>
+    <t xml:space="preserve">1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
+1. For security considerations specific to this guide refer to the  [Privacy, Safety, and Security](security.html) page for requirements and recommendations.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,12 +789,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1221,19 +1215,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
         <v>162</v>
-      </c>
-      <c r="B1" t="s">
-        <v>163</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -1244,13 +1238,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
         <v>164</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>165</v>
-      </c>
-      <c r="E2" t="s">
-        <v>166</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -1261,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" t="s">
         <v>167</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>168</v>
-      </c>
-      <c r="E3" t="s">
-        <v>169</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
@@ -1278,13 +1272,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
         <v>170</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>171</v>
-      </c>
-      <c r="E4" t="s">
-        <v>172</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -2237,10 +2231,10 @@
         <v>19</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -2248,13 +2242,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
         <v>151</v>
-      </c>
-      <c r="B2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" t="s">
-        <v>152</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
@@ -2262,13 +2256,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
         <v>153</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>154</v>
-      </c>
-      <c r="C3" t="s">
-        <v>155</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
@@ -2276,13 +2270,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
         <v>156</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>157</v>
-      </c>
-      <c r="C4" t="s">
-        <v>158</v>
       </c>
       <c r="D4" t="s">
         <v>53</v>
@@ -2290,13 +2284,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" t="s">
         <v>159</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>160</v>
-      </c>
-      <c r="C5" t="s">
-        <v>161</v>
       </c>
       <c r="D5" t="s">
         <v>53</v>
@@ -2315,7 +2309,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2334,63 +2328,63 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
         <v>122</v>
-      </c>
-      <c r="B4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
         <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>126</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" t="s">
         <v>128</v>
-      </c>
-      <c r="B7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" t="s">
         <v>130</v>
-      </c>
-      <c r="B8" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -2408,8 +2402,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2431,23 +2425,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2455,7 +2449,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2463,7 +2457,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2479,7 +2473,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2487,34 +2481,34 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>87</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="s">
         <v>176</v>
-      </c>
-      <c r="B10" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
         <v>178</v>
-      </c>
-      <c r="B11" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2548,7 +2542,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -2559,24 +2553,24 @@
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -2587,95 +2581,95 @@
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>147</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>148</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -2686,16 +2680,16 @@
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2704,13 +2698,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2719,13 +2713,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2734,13 +2728,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2749,13 +2743,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2764,13 +2758,13 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2821,7 +2815,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -2872,21 +2866,21 @@
         <v>80</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -2902,7 +2896,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
@@ -2910,7 +2904,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
         <v>53</v>
@@ -2918,13 +2912,13 @@
     </row>
     <row r="6" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="48" x14ac:dyDescent="0.2">
@@ -2935,73 +2929,73 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="22:25" ht="18" x14ac:dyDescent="0.2">
@@ -3055,19 +3049,19 @@
     </row>
     <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -3105,25 +3099,25 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" t="s">
         <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
         <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I1" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
fix qa prior to publication request
</commit_message>
<xml_diff>
--- a/input/resources-spreadsheets/alert-initiator.xlsx
+++ b/input/resources-spreadsheets/alert-initiator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/davinci-alerts/input/resources-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A114D6-ABFE-6F42-B20D-1D8258D31345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF53D2D7-73B8-D04B-AED5-6B22523C54B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68300" yWindow="500" windowWidth="31900" windowHeight="27460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36620" yWindow="500" windowWidth="31900" windowHeight="27460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="capstatements" sheetId="14" r:id="rId1"/>
@@ -584,9 +584,6 @@
     <t>http://hl7.org/fhir/us/core/STU7/index.html</t>
   </si>
   <si>
-    <t>Da Vinci Health Record Exchange (HRex) 1.1.0 - STU R1</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/davinci-hrex/ImplementationGuide/hl7.fhir.us.davinci-hrex|1.1.0</t>
   </si>
   <si>
@@ -689,6 +686,9 @@
     <t xml:space="preserve">1. For general security consideration refer to the [Security and Privacy Considerations](http://build.fhir.org/secpriv-module.html). 
 1. For security considerations specific to this guide refer to the  [Privacy, Safety, and Security](security.html) page for requirements and recommendations.
 </t>
+  </si>
+  <si>
+    <t>Da Vinci Health Record Exchange (HRex) 1.1.0 - STU 1.1</t>
   </si>
 </sst>
 </file>
@@ -837,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -867,6 +867,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -1215,10 +1216,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
         <v>161</v>
-      </c>
-      <c r="B1" t="s">
-        <v>162</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
@@ -1238,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" t="s">
         <v>163</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>164</v>
-      </c>
-      <c r="E2" t="s">
-        <v>165</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -1255,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s">
         <v>166</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>167</v>
-      </c>
-      <c r="E3" t="s">
-        <v>168</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
@@ -1272,13 +1273,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
         <v>169</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>170</v>
-      </c>
-      <c r="E4" t="s">
-        <v>171</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -2215,8 +2216,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2283,14 +2284,14 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>159</v>
-      </c>
-      <c r="C5" t="s">
-        <v>160</v>
       </c>
       <c r="D5" t="s">
         <v>53</v>
@@ -2331,7 +2332,7 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2339,7 +2340,7 @@
         <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2384,7 +2385,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B9" t="b">
         <v>0</v>
@@ -2402,7 +2403,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2433,7 +2434,7 @@
         <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2481,34 +2482,34 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
         <v>175</v>
-      </c>
-      <c r="B10" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="s">
         <v>177</v>
-      </c>
-      <c r="B11" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="17"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2684,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -2698,7 +2699,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -2713,7 +2714,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -2728,7 +2729,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -2743,7 +2744,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
@@ -2758,7 +2759,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -2866,16 +2867,16 @@
         <v>80</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="16" thickTop="1" x14ac:dyDescent="0.2">

</xml_diff>